<commit_message>
Updates to Trout input files for longer run. Formatting edits for Harp input files.
</commit_message>
<xml_diff>
--- a/HarpLake/HarpLakeparametres.xlsx
+++ b/HarpLake/HarpLakeparametres.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="28455" windowHeight="12525"/>
@@ -117,8 +117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,11 +157,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -269,6 +275,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,231 +451,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>32448</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>32448</v>
+        <v>14.6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>14.6</v>
+        <v>713800</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>713800</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9504293</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>9504293</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>3.7</v>
+        <v>0.37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>0.77</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>0.19</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -678,24 +685,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>